<commit_message>
Update files project version 3.0
Update files project version 3.0
</commit_message>
<xml_diff>
--- a/Project_Manager.xlsx
+++ b/Project_Manager.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/48addad0851d5d47/Máy tính/2023_ChieuT6_CNPM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8C5906-544C-4C5C-8724-96D50C115900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{2E8C5906-544C-4C5C-8724-96D50C115900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B498E103-86CE-4119-95D4-F1B00429357A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>Tuần bắt đầu</t>
   </si>
@@ -116,6 +116,34 @@
   </si>
   <si>
     <t>PHÂN CÔNG CÔNG VIỆC - MILESTONE 2</t>
+  </si>
+  <si>
+    <t>Hoàn thiện các chức năng cuối cùng của project ver3.0 (last version).</t>
+  </si>
+  <si>
+    <t>Thiết kế giao diện cho các chức năng ở milestone 3.</t>
+  </si>
+  <si>
+    <t>Hiện thực các thành phần trên vào code project version 3.0.</t>
+  </si>
+  <si>
+    <t>Hoàn thiện prototypes.</t>
+  </si>
+  <si>
+    <t>Hoàn thiện trigger points.</t>
+  </si>
+  <si>
+    <t>Hoàn thiện screen description.</t>
+  </si>
+  <si>
+    <t>Hạn chót của milestone 3.</t>
+  </si>
+  <si>
+    <t>Thiết kế usecase &amp; sequence diagrams cho các chức năng được
+phân công tiến hành hoàn thiện ở version 3.0 của project.</t>
+  </si>
+  <si>
+    <t>PHÂN CÔNG CÔNG VIỆC - MILESTONE 3</t>
   </si>
 </sst>
 </file>
@@ -304,7 +332,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="45">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -533,8 +561,44 @@
         <bgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-4.9989318521683403E-2"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="48">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -823,37 +887,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1111,11 +1144,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1171,9 +1217,6 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1186,52 +1229,12 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1239,84 +1242,19 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1338,28 +1276,7 @@
     <xf numFmtId="0" fontId="19" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="26" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="28" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1368,40 +1285,13 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="30" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="29" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1413,20 +1303,189 @@
     <xf numFmtId="0" fontId="19" fillId="37" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="38" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="41" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="42" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="39" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="43" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="40" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="44" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="44" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1674,7 +1733,7 @@
   <dimension ref="A1:AI28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1703,40 +1762,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="33.75" customHeight="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="48"/>
-      <c r="T1" s="48"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="48"/>
-      <c r="W1" s="48"/>
-      <c r="X1" s="48"/>
-      <c r="Y1" s="48"/>
-      <c r="Z1" s="48"/>
-      <c r="AA1" s="51" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="34"/>
+      <c r="AA1" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="51"/>
+      <c r="AB1" s="81"/>
+      <c r="AC1" s="81"/>
+      <c r="AD1" s="81"/>
       <c r="AE1" s="2"/>
       <c r="AF1" s="3"/>
     </row>
@@ -1768,24 +1804,24 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
-      <c r="AB2" s="37"/>
-      <c r="AC2" s="35"/>
-      <c r="AD2" s="35"/>
+      <c r="AB2" s="108"/>
+      <c r="AC2" s="106"/>
+      <c r="AD2" s="106"/>
       <c r="AE2" s="1"/>
       <c r="AF2" s="6"/>
     </row>
     <row r="3" spans="1:35" ht="21" customHeight="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41">
+      <c r="B3" s="110"/>
+      <c r="C3" s="111"/>
+      <c r="D3" s="112">
         <v>45023</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="43"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="114"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -1808,9 +1844,9 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="34"/>
-      <c r="AC3" s="35"/>
-      <c r="AD3" s="35"/>
+      <c r="AB3" s="105"/>
+      <c r="AC3" s="106"/>
+      <c r="AD3" s="106"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="8"/>
     </row>
@@ -1941,7 +1977,7 @@
       <c r="AF5" s="15"/>
     </row>
     <row r="6" spans="1:35" ht="18" customHeight="1" thickBot="1">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="115" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="16">
@@ -2063,7 +2099,7 @@
       <c r="AF6" s="19"/>
     </row>
     <row r="7" spans="1:35" ht="18" customHeight="1">
-      <c r="A7" s="45"/>
+      <c r="A7" s="116"/>
       <c r="B7" s="20">
         <f t="shared" ref="B7:P7" si="2">B6</f>
         <v>45023</v>
@@ -2178,720 +2214,720 @@
       </c>
       <c r="AD7" s="22"/>
       <c r="AE7" s="14"/>
-      <c r="AF7" s="67" t="s">
+      <c r="AF7" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="AG7" s="68"/>
-      <c r="AH7" s="68"/>
-      <c r="AI7" s="69"/>
+      <c r="AG7" s="86"/>
+      <c r="AH7" s="86"/>
+      <c r="AI7" s="87"/>
     </row>
     <row r="8" spans="1:35" ht="21" customHeight="1">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="93"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="57"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="57"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="57"/>
-      <c r="V8" s="25"/>
-      <c r="W8" s="57"/>
-      <c r="X8" s="25"/>
-      <c r="Y8" s="24"/>
-      <c r="Z8" s="25"/>
-      <c r="AA8" s="24"/>
-      <c r="AB8" s="25"/>
-      <c r="AC8" s="24"/>
-      <c r="AD8" s="26"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="36"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="36"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="36"/>
+      <c r="V8" s="24"/>
+      <c r="W8" s="36"/>
+      <c r="X8" s="24"/>
+      <c r="Y8" s="23"/>
+      <c r="Z8" s="24"/>
+      <c r="AA8" s="23"/>
+      <c r="AB8" s="24"/>
+      <c r="AC8" s="23"/>
+      <c r="AD8" s="25"/>
       <c r="AE8" s="1"/>
-      <c r="AF8" s="73"/>
-      <c r="AG8" s="74"/>
-      <c r="AH8" s="74"/>
-      <c r="AI8" s="75"/>
+      <c r="AF8" s="88"/>
+      <c r="AG8" s="89"/>
+      <c r="AH8" s="89"/>
+      <c r="AI8" s="90"/>
     </row>
     <row r="9" spans="1:35" ht="21" customHeight="1">
-      <c r="A9" s="55"/>
-      <c r="B9" s="97"/>
-      <c r="C9" s="98"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="58"/>
-      <c r="R9" s="27"/>
-      <c r="S9" s="58"/>
-      <c r="T9" s="27"/>
-      <c r="U9" s="58"/>
-      <c r="V9" s="27"/>
-      <c r="W9" s="58"/>
-      <c r="X9" s="27"/>
-      <c r="Y9" s="28"/>
-      <c r="Z9" s="27"/>
-      <c r="AA9" s="28"/>
-      <c r="AB9" s="27"/>
-      <c r="AC9" s="28"/>
-      <c r="AD9" s="29"/>
+      <c r="A9" s="83"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="26"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="26"/>
+      <c r="U9" s="37"/>
+      <c r="V9" s="26"/>
+      <c r="W9" s="37"/>
+      <c r="X9" s="26"/>
+      <c r="Y9" s="27"/>
+      <c r="Z9" s="26"/>
+      <c r="AA9" s="27"/>
+      <c r="AB9" s="26"/>
+      <c r="AC9" s="27"/>
+      <c r="AD9" s="28"/>
       <c r="AE9" s="1"/>
-      <c r="AF9" s="85"/>
-      <c r="AG9" s="76" t="s">
+      <c r="AF9" s="40"/>
+      <c r="AG9" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="AH9" s="77"/>
-      <c r="AI9" s="80"/>
+      <c r="AH9" s="98"/>
+      <c r="AI9" s="99"/>
     </row>
     <row r="10" spans="1:35" ht="21" customHeight="1">
-      <c r="A10" s="55"/>
-      <c r="B10" s="99"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="58"/>
-      <c r="R10" s="27"/>
-      <c r="S10" s="58"/>
-      <c r="T10" s="27"/>
-      <c r="U10" s="58"/>
-      <c r="V10" s="27"/>
-      <c r="W10" s="58"/>
-      <c r="X10" s="27"/>
-      <c r="Y10" s="28"/>
-      <c r="Z10" s="27"/>
-      <c r="AA10" s="28"/>
-      <c r="AB10" s="27"/>
-      <c r="AC10" s="28"/>
-      <c r="AD10" s="29"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="37"/>
+      <c r="R10" s="26"/>
+      <c r="S10" s="37"/>
+      <c r="T10" s="26"/>
+      <c r="U10" s="37"/>
+      <c r="V10" s="26"/>
+      <c r="W10" s="37"/>
+      <c r="X10" s="26"/>
+      <c r="Y10" s="27"/>
+      <c r="Z10" s="26"/>
+      <c r="AA10" s="27"/>
+      <c r="AB10" s="26"/>
+      <c r="AC10" s="27"/>
+      <c r="AD10" s="28"/>
       <c r="AE10" s="1"/>
-      <c r="AF10" s="86"/>
-      <c r="AG10" s="76" t="s">
+      <c r="AF10" s="41"/>
+      <c r="AG10" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="AH10" s="77"/>
-      <c r="AI10" s="80"/>
+      <c r="AH10" s="98"/>
+      <c r="AI10" s="99"/>
     </row>
     <row r="11" spans="1:35" ht="21" customHeight="1">
-      <c r="A11" s="55"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="101"/>
-      <c r="D11" s="100"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="101"/>
-      <c r="H11" s="119"/>
-      <c r="I11" s="120"/>
-      <c r="J11" s="119"/>
-      <c r="K11" s="120"/>
-      <c r="L11" s="119"/>
-      <c r="M11" s="120"/>
-      <c r="N11" s="119"/>
-      <c r="O11" s="120"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="59"/>
-      <c r="R11" s="30"/>
-      <c r="S11" s="59"/>
-      <c r="T11" s="30"/>
-      <c r="U11" s="59"/>
-      <c r="V11" s="30"/>
-      <c r="W11" s="59"/>
-      <c r="X11" s="30"/>
-      <c r="Y11" s="28"/>
-      <c r="Z11" s="30"/>
-      <c r="AA11" s="28"/>
-      <c r="AB11" s="30"/>
-      <c r="AC11" s="28"/>
-      <c r="AD11" s="29"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="67"/>
+      <c r="N11" s="66"/>
+      <c r="O11" s="67"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="29"/>
+      <c r="S11" s="38"/>
+      <c r="T11" s="29"/>
+      <c r="U11" s="38"/>
+      <c r="V11" s="29"/>
+      <c r="W11" s="38"/>
+      <c r="X11" s="29"/>
+      <c r="Y11" s="27"/>
+      <c r="Z11" s="29"/>
+      <c r="AA11" s="27"/>
+      <c r="AB11" s="29"/>
+      <c r="AC11" s="27"/>
+      <c r="AD11" s="28"/>
       <c r="AE11" s="1"/>
-      <c r="AF11" s="87"/>
-      <c r="AG11" s="76" t="s">
+      <c r="AF11" s="42"/>
+      <c r="AG11" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="AH11" s="77"/>
-      <c r="AI11" s="80"/>
+      <c r="AH11" s="98"/>
+      <c r="AI11" s="99"/>
     </row>
     <row r="12" spans="1:35" ht="21" customHeight="1">
-      <c r="A12" s="55"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="109"/>
-      <c r="E12" s="102"/>
-      <c r="F12" s="109"/>
-      <c r="G12" s="102"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="58"/>
-      <c r="R12" s="27"/>
-      <c r="S12" s="58"/>
-      <c r="T12" s="27"/>
-      <c r="U12" s="58"/>
-      <c r="V12" s="27"/>
-      <c r="W12" s="58"/>
-      <c r="X12" s="27"/>
-      <c r="Y12" s="28"/>
-      <c r="Z12" s="27"/>
-      <c r="AA12" s="28"/>
-      <c r="AB12" s="27"/>
-      <c r="AC12" s="28"/>
-      <c r="AD12" s="29"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="26"/>
+      <c r="S12" s="37"/>
+      <c r="T12" s="26"/>
+      <c r="U12" s="37"/>
+      <c r="V12" s="26"/>
+      <c r="W12" s="37"/>
+      <c r="X12" s="26"/>
+      <c r="Y12" s="27"/>
+      <c r="Z12" s="26"/>
+      <c r="AA12" s="27"/>
+      <c r="AB12" s="26"/>
+      <c r="AC12" s="27"/>
+      <c r="AD12" s="28"/>
       <c r="AE12" s="1"/>
-      <c r="AF12" s="88"/>
-      <c r="AG12" s="78" t="s">
+      <c r="AF12" s="43"/>
+      <c r="AG12" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="AH12" s="79"/>
-      <c r="AI12" s="81"/>
+      <c r="AH12" s="98"/>
+      <c r="AI12" s="99"/>
     </row>
     <row r="13" spans="1:35" ht="21" customHeight="1">
-      <c r="A13" s="55"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="121"/>
-      <c r="E13" s="120"/>
-      <c r="F13" s="121"/>
-      <c r="G13" s="120"/>
-      <c r="H13" s="105"/>
-      <c r="I13" s="106"/>
-      <c r="J13" s="105"/>
-      <c r="K13" s="106"/>
-      <c r="L13" s="105"/>
-      <c r="M13" s="106"/>
-      <c r="N13" s="105"/>
-      <c r="O13" s="106"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="58"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="58"/>
-      <c r="T13" s="27"/>
-      <c r="U13" s="58"/>
-      <c r="V13" s="27"/>
-      <c r="W13" s="58"/>
-      <c r="X13" s="27"/>
-      <c r="Y13" s="28"/>
-      <c r="Z13" s="27"/>
-      <c r="AA13" s="28"/>
-      <c r="AB13" s="27"/>
-      <c r="AC13" s="28"/>
-      <c r="AD13" s="29"/>
+      <c r="A13" s="83"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="59"/>
+      <c r="M13" s="60"/>
+      <c r="N13" s="59"/>
+      <c r="O13" s="60"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="37"/>
+      <c r="T13" s="26"/>
+      <c r="U13" s="37"/>
+      <c r="V13" s="26"/>
+      <c r="W13" s="37"/>
+      <c r="X13" s="26"/>
+      <c r="Y13" s="27"/>
+      <c r="Z13" s="26"/>
+      <c r="AA13" s="27"/>
+      <c r="AB13" s="26"/>
+      <c r="AC13" s="27"/>
+      <c r="AD13" s="28"/>
       <c r="AE13" s="1"/>
-      <c r="AF13" s="89"/>
-      <c r="AG13" s="78" t="s">
+      <c r="AF13" s="44"/>
+      <c r="AG13" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="AH13" s="79"/>
-      <c r="AI13" s="81"/>
+      <c r="AH13" s="98"/>
+      <c r="AI13" s="99"/>
     </row>
     <row r="14" spans="1:35" ht="21" customHeight="1">
-      <c r="A14" s="55"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="121"/>
-      <c r="E14" s="120"/>
-      <c r="F14" s="121"/>
-      <c r="G14" s="120"/>
-      <c r="H14" s="103"/>
-      <c r="I14" s="104"/>
-      <c r="J14" s="103"/>
-      <c r="K14" s="104"/>
-      <c r="L14" s="103"/>
-      <c r="M14" s="104"/>
-      <c r="N14" s="103"/>
-      <c r="O14" s="104"/>
-      <c r="P14" s="103"/>
-      <c r="Q14" s="103"/>
-      <c r="R14" s="103"/>
-      <c r="S14" s="103"/>
-      <c r="T14" s="103"/>
-      <c r="U14" s="103"/>
-      <c r="V14" s="103"/>
-      <c r="W14" s="103"/>
-      <c r="X14" s="103"/>
-      <c r="Y14" s="104"/>
-      <c r="Z14" s="103"/>
-      <c r="AA14" s="104"/>
-      <c r="AB14" s="103"/>
-      <c r="AC14" s="28"/>
-      <c r="AD14" s="29"/>
+      <c r="A14" s="83"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="57"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="57"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="57"/>
+      <c r="Q14" s="57"/>
+      <c r="R14" s="57"/>
+      <c r="S14" s="57"/>
+      <c r="T14" s="57"/>
+      <c r="U14" s="57"/>
+      <c r="V14" s="57"/>
+      <c r="W14" s="57"/>
+      <c r="X14" s="57"/>
+      <c r="Y14" s="58"/>
+      <c r="Z14" s="57"/>
+      <c r="AA14" s="58"/>
+      <c r="AB14" s="57"/>
+      <c r="AC14" s="27"/>
+      <c r="AD14" s="28"/>
       <c r="AE14" s="1"/>
-      <c r="AF14" s="90"/>
-      <c r="AG14" s="78" t="s">
+      <c r="AF14" s="45"/>
+      <c r="AG14" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="AH14" s="79"/>
-      <c r="AI14" s="81"/>
+      <c r="AH14" s="98"/>
+      <c r="AI14" s="99"/>
     </row>
     <row r="15" spans="1:35" ht="21" customHeight="1">
-      <c r="A15" s="55"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="121"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="121"/>
-      <c r="G15" s="120"/>
-      <c r="H15" s="107"/>
-      <c r="I15" s="108"/>
-      <c r="J15" s="107"/>
-      <c r="K15" s="108"/>
-      <c r="L15" s="107"/>
-      <c r="M15" s="108"/>
-      <c r="N15" s="107"/>
-      <c r="O15" s="108"/>
-      <c r="P15" s="107"/>
-      <c r="Q15" s="107"/>
-      <c r="R15" s="107"/>
-      <c r="S15" s="107"/>
-      <c r="T15" s="107"/>
-      <c r="U15" s="107"/>
-      <c r="V15" s="107"/>
-      <c r="W15" s="107"/>
-      <c r="X15" s="107"/>
-      <c r="Y15" s="108"/>
-      <c r="Z15" s="107"/>
-      <c r="AA15" s="108"/>
-      <c r="AB15" s="107"/>
-      <c r="AC15" s="28"/>
-      <c r="AD15" s="29"/>
+      <c r="A15" s="83"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="62"/>
+      <c r="L15" s="61"/>
+      <c r="M15" s="62"/>
+      <c r="N15" s="61"/>
+      <c r="O15" s="62"/>
+      <c r="P15" s="61"/>
+      <c r="Q15" s="61"/>
+      <c r="R15" s="61"/>
+      <c r="S15" s="61"/>
+      <c r="T15" s="61"/>
+      <c r="U15" s="61"/>
+      <c r="V15" s="61"/>
+      <c r="W15" s="61"/>
+      <c r="X15" s="61"/>
+      <c r="Y15" s="62"/>
+      <c r="Z15" s="61"/>
+      <c r="AA15" s="62"/>
+      <c r="AB15" s="61"/>
+      <c r="AC15" s="27"/>
+      <c r="AD15" s="28"/>
       <c r="AE15" s="1"/>
-      <c r="AF15" s="91"/>
-      <c r="AG15" s="78" t="s">
+      <c r="AF15" s="46"/>
+      <c r="AG15" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="AH15" s="79"/>
-      <c r="AI15" s="81"/>
+      <c r="AH15" s="98"/>
+      <c r="AI15" s="99"/>
     </row>
     <row r="16" spans="1:35" ht="21" customHeight="1">
-      <c r="A16" s="55"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="58"/>
-      <c r="R16" s="27"/>
-      <c r="S16" s="58"/>
-      <c r="T16" s="27"/>
-      <c r="U16" s="58"/>
-      <c r="V16" s="27"/>
-      <c r="W16" s="58"/>
-      <c r="X16" s="27"/>
-      <c r="Y16" s="28"/>
-      <c r="Z16" s="27"/>
-      <c r="AA16" s="28"/>
-      <c r="AB16" s="27"/>
-      <c r="AC16" s="118" t="s">
+      <c r="A16" s="83"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="37"/>
+      <c r="R16" s="26"/>
+      <c r="S16" s="37"/>
+      <c r="T16" s="26"/>
+      <c r="U16" s="37"/>
+      <c r="V16" s="26"/>
+      <c r="W16" s="37"/>
+      <c r="X16" s="26"/>
+      <c r="Y16" s="27"/>
+      <c r="Z16" s="26"/>
+      <c r="AA16" s="27"/>
+      <c r="AB16" s="26"/>
+      <c r="AC16" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="AD16" s="29"/>
+      <c r="AD16" s="28"/>
       <c r="AE16" s="1"/>
-      <c r="AF16" s="92"/>
-      <c r="AG16" s="82" t="s">
+      <c r="AF16" s="100"/>
+      <c r="AG16" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="AH16" s="83"/>
-      <c r="AI16" s="84"/>
+      <c r="AH16" s="92"/>
+      <c r="AI16" s="93"/>
     </row>
     <row r="17" spans="1:35" ht="21" customHeight="1">
-      <c r="A17" s="55"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="58"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="58"/>
-      <c r="T17" s="27"/>
-      <c r="U17" s="58"/>
-      <c r="V17" s="27"/>
-      <c r="W17" s="58"/>
-      <c r="X17" s="27"/>
-      <c r="Y17" s="28"/>
-      <c r="Z17" s="27"/>
-      <c r="AA17" s="28"/>
-      <c r="AB17" s="27"/>
-      <c r="AC17" s="28"/>
-      <c r="AD17" s="29"/>
+      <c r="A17" s="83"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="26"/>
+      <c r="S17" s="37"/>
+      <c r="T17" s="26"/>
+      <c r="U17" s="37"/>
+      <c r="V17" s="26"/>
+      <c r="W17" s="37"/>
+      <c r="X17" s="26"/>
+      <c r="Y17" s="27"/>
+      <c r="Z17" s="26"/>
+      <c r="AA17" s="27"/>
+      <c r="AB17" s="26"/>
+      <c r="AC17" s="27"/>
+      <c r="AD17" s="28"/>
       <c r="AE17" s="1"/>
-      <c r="AF17" s="110"/>
-      <c r="AG17" s="111"/>
-      <c r="AH17" s="112"/>
-      <c r="AI17" s="113"/>
+      <c r="AF17" s="101"/>
+      <c r="AG17" s="94"/>
+      <c r="AH17" s="95"/>
+      <c r="AI17" s="96"/>
     </row>
     <row r="18" spans="1:35" ht="21" customHeight="1" thickBot="1">
-      <c r="A18" s="55"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="58"/>
-      <c r="R18" s="27"/>
-      <c r="S18" s="58"/>
-      <c r="T18" s="27"/>
-      <c r="U18" s="58"/>
-      <c r="V18" s="27"/>
-      <c r="W18" s="58"/>
-      <c r="X18" s="27"/>
-      <c r="Y18" s="28"/>
-      <c r="Z18" s="27"/>
-      <c r="AA18" s="28"/>
-      <c r="AB18" s="27"/>
-      <c r="AC18" s="28"/>
-      <c r="AD18" s="29"/>
+      <c r="A18" s="83"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="37"/>
+      <c r="R18" s="26"/>
+      <c r="S18" s="37"/>
+      <c r="T18" s="26"/>
+      <c r="U18" s="37"/>
+      <c r="V18" s="26"/>
+      <c r="W18" s="37"/>
+      <c r="X18" s="26"/>
+      <c r="Y18" s="27"/>
+      <c r="Z18" s="26"/>
+      <c r="AA18" s="27"/>
+      <c r="AB18" s="26"/>
+      <c r="AC18" s="27"/>
+      <c r="AD18" s="28"/>
       <c r="AE18" s="1"/>
-      <c r="AF18" s="114"/>
-      <c r="AG18" s="115" t="s">
+      <c r="AF18" s="64"/>
+      <c r="AG18" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="AH18" s="116"/>
-      <c r="AI18" s="117"/>
+      <c r="AH18" s="103"/>
+      <c r="AI18" s="104"/>
     </row>
     <row r="19" spans="1:35" ht="21" customHeight="1">
-      <c r="A19" s="55"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="27"/>
-      <c r="Q19" s="58"/>
-      <c r="R19" s="27"/>
-      <c r="S19" s="58"/>
-      <c r="T19" s="27"/>
-      <c r="U19" s="58"/>
-      <c r="V19" s="27"/>
-      <c r="W19" s="58"/>
-      <c r="X19" s="27"/>
-      <c r="Y19" s="28"/>
-      <c r="Z19" s="27"/>
-      <c r="AA19" s="28"/>
-      <c r="AB19" s="27"/>
-      <c r="AC19" s="28"/>
-      <c r="AD19" s="29"/>
+      <c r="A19" s="83"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="37"/>
+      <c r="T19" s="26"/>
+      <c r="U19" s="37"/>
+      <c r="V19" s="26"/>
+      <c r="W19" s="37"/>
+      <c r="X19" s="26"/>
+      <c r="Y19" s="27"/>
+      <c r="Z19" s="26"/>
+      <c r="AA19" s="27"/>
+      <c r="AB19" s="26"/>
+      <c r="AC19" s="27"/>
+      <c r="AD19" s="28"/>
       <c r="AE19" s="1"/>
-      <c r="AF19" s="53"/>
-      <c r="AG19" s="53"/>
-      <c r="AH19" s="53"/>
-      <c r="AI19" s="53"/>
+      <c r="AF19" s="1"/>
+      <c r="AG19" s="1"/>
+      <c r="AH19" s="1"/>
+      <c r="AI19" s="1"/>
     </row>
     <row r="20" spans="1:35" ht="21" customHeight="1">
-      <c r="A20" s="55"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="27"/>
-      <c r="Q20" s="58"/>
-      <c r="R20" s="27"/>
-      <c r="S20" s="58"/>
-      <c r="T20" s="27"/>
-      <c r="U20" s="58"/>
-      <c r="V20" s="27"/>
-      <c r="W20" s="58"/>
-      <c r="X20" s="27"/>
-      <c r="Y20" s="28"/>
-      <c r="Z20" s="27"/>
-      <c r="AA20" s="28"/>
-      <c r="AB20" s="27"/>
-      <c r="AC20" s="28"/>
-      <c r="AD20" s="29"/>
+      <c r="A20" s="83"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="26"/>
+      <c r="Q20" s="37"/>
+      <c r="R20" s="26"/>
+      <c r="S20" s="37"/>
+      <c r="T20" s="26"/>
+      <c r="U20" s="37"/>
+      <c r="V20" s="26"/>
+      <c r="W20" s="37"/>
+      <c r="X20" s="26"/>
+      <c r="Y20" s="27"/>
+      <c r="Z20" s="26"/>
+      <c r="AA20" s="27"/>
+      <c r="AB20" s="26"/>
+      <c r="AC20" s="27"/>
+      <c r="AD20" s="28"/>
       <c r="AE20" s="1"/>
-      <c r="AF20" s="53"/>
-      <c r="AG20" s="53"/>
-      <c r="AH20" s="53"/>
-      <c r="AI20" s="53"/>
+      <c r="AF20" s="1"/>
+      <c r="AG20" s="1"/>
+      <c r="AH20" s="1"/>
+      <c r="AI20" s="1"/>
     </row>
     <row r="21" spans="1:35" ht="21" customHeight="1">
-      <c r="A21" s="55"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="28"/>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="58"/>
-      <c r="R21" s="27"/>
-      <c r="S21" s="58"/>
-      <c r="T21" s="27"/>
-      <c r="U21" s="58"/>
-      <c r="V21" s="27"/>
-      <c r="W21" s="58"/>
-      <c r="X21" s="27"/>
-      <c r="Y21" s="28"/>
-      <c r="Z21" s="27"/>
-      <c r="AA21" s="28"/>
-      <c r="AB21" s="27"/>
-      <c r="AC21" s="28"/>
-      <c r="AD21" s="29"/>
+      <c r="A21" s="83"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="37"/>
+      <c r="R21" s="26"/>
+      <c r="S21" s="37"/>
+      <c r="T21" s="26"/>
+      <c r="U21" s="37"/>
+      <c r="V21" s="26"/>
+      <c r="W21" s="37"/>
+      <c r="X21" s="26"/>
+      <c r="Y21" s="27"/>
+      <c r="Z21" s="26"/>
+      <c r="AA21" s="27"/>
+      <c r="AB21" s="26"/>
+      <c r="AC21" s="27"/>
+      <c r="AD21" s="28"/>
       <c r="AE21" s="1"/>
-      <c r="AF21" s="53"/>
-      <c r="AG21" s="53"/>
-      <c r="AH21" s="53"/>
-      <c r="AI21" s="53"/>
+      <c r="AF21" s="1"/>
+      <c r="AG21" s="1"/>
+      <c r="AH21" s="1"/>
+      <c r="AI21" s="1"/>
     </row>
     <row r="22" spans="1:35" ht="21" customHeight="1">
-      <c r="A22" s="55"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="58"/>
-      <c r="R22" s="27"/>
-      <c r="S22" s="58"/>
-      <c r="T22" s="27"/>
-      <c r="U22" s="58"/>
-      <c r="V22" s="27"/>
-      <c r="W22" s="58"/>
-      <c r="X22" s="27"/>
-      <c r="Y22" s="28"/>
-      <c r="Z22" s="27"/>
-      <c r="AA22" s="28"/>
-      <c r="AB22" s="27"/>
-      <c r="AC22" s="28"/>
-      <c r="AD22" s="29"/>
+      <c r="A22" s="83"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="37"/>
+      <c r="R22" s="26"/>
+      <c r="S22" s="37"/>
+      <c r="T22" s="26"/>
+      <c r="U22" s="37"/>
+      <c r="V22" s="26"/>
+      <c r="W22" s="37"/>
+      <c r="X22" s="26"/>
+      <c r="Y22" s="27"/>
+      <c r="Z22" s="26"/>
+      <c r="AA22" s="27"/>
+      <c r="AB22" s="26"/>
+      <c r="AC22" s="27"/>
+      <c r="AD22" s="28"/>
       <c r="AE22" s="1"/>
       <c r="AF22" s="1"/>
     </row>
     <row r="23" spans="1:35" ht="21" customHeight="1">
-      <c r="A23" s="55"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="28"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="58"/>
-      <c r="R23" s="27"/>
-      <c r="S23" s="58"/>
-      <c r="T23" s="27"/>
-      <c r="U23" s="58"/>
-      <c r="V23" s="27"/>
-      <c r="W23" s="58"/>
-      <c r="X23" s="27"/>
-      <c r="Y23" s="28"/>
-      <c r="Z23" s="27"/>
-      <c r="AA23" s="28"/>
-      <c r="AB23" s="27"/>
-      <c r="AC23" s="28"/>
-      <c r="AD23" s="29"/>
+      <c r="A23" s="83"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="37"/>
+      <c r="R23" s="26"/>
+      <c r="S23" s="37"/>
+      <c r="T23" s="26"/>
+      <c r="U23" s="37"/>
+      <c r="V23" s="26"/>
+      <c r="W23" s="37"/>
+      <c r="X23" s="26"/>
+      <c r="Y23" s="27"/>
+      <c r="Z23" s="26"/>
+      <c r="AA23" s="27"/>
+      <c r="AB23" s="26"/>
+      <c r="AC23" s="27"/>
+      <c r="AD23" s="28"/>
       <c r="AE23" s="1"/>
       <c r="AF23" s="1"/>
     </row>
     <row r="24" spans="1:35" ht="21" customHeight="1">
-      <c r="A24" s="55"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="28"/>
-      <c r="P24" s="27"/>
-      <c r="Q24" s="58"/>
-      <c r="R24" s="27"/>
-      <c r="S24" s="58"/>
-      <c r="T24" s="27"/>
-      <c r="U24" s="58"/>
-      <c r="V24" s="27"/>
-      <c r="W24" s="58"/>
-      <c r="X24" s="27"/>
-      <c r="Y24" s="28"/>
-      <c r="Z24" s="27"/>
-      <c r="AA24" s="28"/>
-      <c r="AB24" s="27"/>
-      <c r="AC24" s="28"/>
-      <c r="AD24" s="29"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="26"/>
+      <c r="Q24" s="37"/>
+      <c r="R24" s="26"/>
+      <c r="S24" s="37"/>
+      <c r="T24" s="26"/>
+      <c r="U24" s="37"/>
+      <c r="V24" s="26"/>
+      <c r="W24" s="37"/>
+      <c r="X24" s="26"/>
+      <c r="Y24" s="27"/>
+      <c r="Z24" s="26"/>
+      <c r="AA24" s="27"/>
+      <c r="AB24" s="26"/>
+      <c r="AC24" s="27"/>
+      <c r="AD24" s="28"/>
       <c r="AE24" s="1"/>
       <c r="AF24" s="1"/>
     </row>
     <row r="25" spans="1:35" ht="21" customHeight="1">
-      <c r="A25" s="55"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="27"/>
-      <c r="O25" s="28"/>
-      <c r="P25" s="27"/>
-      <c r="Q25" s="58"/>
-      <c r="R25" s="27"/>
-      <c r="S25" s="58"/>
-      <c r="T25" s="27"/>
-      <c r="U25" s="58"/>
-      <c r="V25" s="27"/>
-      <c r="W25" s="58"/>
-      <c r="X25" s="27"/>
-      <c r="Y25" s="28"/>
-      <c r="Z25" s="27"/>
-      <c r="AA25" s="28"/>
-      <c r="AB25" s="27"/>
-      <c r="AC25" s="28"/>
-      <c r="AD25" s="29"/>
+      <c r="A25" s="83"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="26"/>
+      <c r="Q25" s="37"/>
+      <c r="R25" s="26"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="26"/>
+      <c r="U25" s="37"/>
+      <c r="V25" s="26"/>
+      <c r="W25" s="37"/>
+      <c r="X25" s="26"/>
+      <c r="Y25" s="27"/>
+      <c r="Z25" s="26"/>
+      <c r="AA25" s="27"/>
+      <c r="AB25" s="26"/>
+      <c r="AC25" s="27"/>
+      <c r="AD25" s="28"/>
       <c r="AE25" s="1"/>
       <c r="AF25" s="1"/>
     </row>
     <row r="26" spans="1:35" ht="21" customHeight="1">
-      <c r="A26" s="56"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="32"/>
-      <c r="P26" s="31"/>
-      <c r="Q26" s="60"/>
-      <c r="R26" s="31"/>
-      <c r="S26" s="60"/>
-      <c r="T26" s="31"/>
-      <c r="U26" s="60"/>
-      <c r="V26" s="31"/>
-      <c r="W26" s="60"/>
-      <c r="X26" s="31"/>
-      <c r="Y26" s="32"/>
-      <c r="Z26" s="31"/>
-      <c r="AA26" s="32"/>
-      <c r="AB26" s="31"/>
-      <c r="AC26" s="32"/>
-      <c r="AD26" s="33"/>
+      <c r="A26" s="84"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="31"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="39"/>
+      <c r="R26" s="30"/>
+      <c r="S26" s="39"/>
+      <c r="T26" s="30"/>
+      <c r="U26" s="39"/>
+      <c r="V26" s="30"/>
+      <c r="W26" s="39"/>
+      <c r="X26" s="30"/>
+      <c r="Y26" s="31"/>
+      <c r="Z26" s="30"/>
+      <c r="AA26" s="31"/>
+      <c r="AB26" s="30"/>
+      <c r="AC26" s="31"/>
+      <c r="AD26" s="32"/>
       <c r="AE26" s="1"/>
       <c r="AF26" s="1"/>
     </row>
@@ -2955,19 +2991,24 @@
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
       <c r="Y28" s="1"/>
-      <c r="Z28" s="36" t="str">
+      <c r="Z28" s="107" t="str">
         <f>HYPERLINK("https://www.vertex42.com/ExcelTemplates/project-schedule-template.html","Project Schedule Template © 2014-2019 by Vertex42.com")</f>
         <v>Project Schedule Template © 2014-2019 by Vertex42.com</v>
       </c>
-      <c r="AA28" s="35"/>
-      <c r="AB28" s="35"/>
-      <c r="AC28" s="35"/>
-      <c r="AD28" s="35"/>
+      <c r="AA28" s="106"/>
+      <c r="AB28" s="106"/>
+      <c r="AC28" s="106"/>
+      <c r="AD28" s="106"/>
       <c r="AE28" s="1"/>
       <c r="AF28" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="Z28:AD28"/>
+    <mergeCell ref="AB2:AD2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="A6:A7"/>
     <mergeCell ref="AA1:AD1"/>
     <mergeCell ref="A8:A26"/>
     <mergeCell ref="AF7:AI8"/>
@@ -2982,11 +3023,6 @@
     <mergeCell ref="AF16:AF17"/>
     <mergeCell ref="AG18:AI18"/>
     <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="Z28:AD28"/>
-    <mergeCell ref="AB2:AD2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <conditionalFormatting sqref="M5">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Vertex42">
@@ -3007,7 +3043,7 @@
   <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -3029,24 +3065,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="50"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="34"/>
+      <c r="P1" s="35"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="3"/>
     </row>
@@ -3070,17 +3094,17 @@
       <c r="R2" s="6"/>
     </row>
     <row r="3" spans="1:21" ht="21" customHeight="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41">
+      <c r="B3" s="110"/>
+      <c r="C3" s="111"/>
+      <c r="D3" s="112">
         <v>45051</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="43"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="114"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -3165,7 +3189,7 @@
       <c r="R5" s="15"/>
     </row>
     <row r="6" spans="1:21" ht="18" customHeight="1">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="115" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="16">
@@ -3231,7 +3255,7 @@
       <c r="R6" s="19"/>
     </row>
     <row r="7" spans="1:21" ht="18" customHeight="1" thickBot="1">
-      <c r="A7" s="45"/>
+      <c r="A7" s="116"/>
       <c r="B7" s="20">
         <f t="shared" ref="B7:O7" si="1">B6</f>
         <v>45051</v>
@@ -3293,441 +3317,429 @@
       <c r="R7" s="19"/>
     </row>
     <row r="8" spans="1:21" ht="21" customHeight="1">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="134"/>
-      <c r="C8" s="135"/>
-      <c r="D8" s="136"/>
-      <c r="E8" s="135"/>
-      <c r="F8" s="136"/>
-      <c r="G8" s="135"/>
-      <c r="H8" s="136"/>
-      <c r="I8" s="135"/>
-      <c r="J8" s="136"/>
-      <c r="K8" s="135"/>
-      <c r="L8" s="136"/>
-      <c r="M8" s="135"/>
-      <c r="N8" s="136"/>
-      <c r="O8" s="135"/>
-      <c r="P8" s="26"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="73"/>
+      <c r="N8" s="74"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="25"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="123" t="s">
+      <c r="R8" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="S8" s="124"/>
-      <c r="T8" s="124"/>
-      <c r="U8" s="125"/>
+      <c r="S8" s="118"/>
+      <c r="T8" s="118"/>
+      <c r="U8" s="119"/>
     </row>
     <row r="9" spans="1:21" ht="21" customHeight="1">
-      <c r="A9" s="55"/>
-      <c r="B9" s="95"/>
-      <c r="C9" s="96"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="96"/>
-      <c r="F9" s="95"/>
-      <c r="G9" s="96"/>
-      <c r="H9" s="95"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="29"/>
+      <c r="A9" s="83"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="28"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="126"/>
-      <c r="S9" s="122"/>
-      <c r="T9" s="122"/>
-      <c r="U9" s="127"/>
+      <c r="R9" s="120"/>
+      <c r="S9" s="121"/>
+      <c r="T9" s="121"/>
+      <c r="U9" s="122"/>
     </row>
     <row r="10" spans="1:21" ht="21" customHeight="1">
-      <c r="A10" s="55"/>
-      <c r="B10" s="97"/>
-      <c r="C10" s="98"/>
-      <c r="D10" s="97"/>
-      <c r="E10" s="98"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="29"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="28"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="128"/>
-      <c r="S10" s="133" t="s">
+      <c r="R10" s="69"/>
+      <c r="S10" s="127" t="s">
         <v>21</v>
       </c>
-      <c r="T10" s="131"/>
-      <c r="U10" s="132"/>
+      <c r="T10" s="128"/>
+      <c r="U10" s="129"/>
     </row>
     <row r="11" spans="1:21" ht="21" customHeight="1">
-      <c r="A11" s="55"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="137"/>
-      <c r="G11" s="138"/>
-      <c r="H11" s="137"/>
-      <c r="I11" s="138"/>
-      <c r="J11" s="137"/>
-      <c r="K11" s="138"/>
-      <c r="L11" s="137"/>
-      <c r="M11" s="138"/>
-      <c r="N11" s="137"/>
-      <c r="O11" s="138"/>
-      <c r="P11" s="29"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="76"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="75"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="75"/>
+      <c r="O11" s="76"/>
+      <c r="P11" s="28"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="85"/>
-      <c r="S11" s="133" t="s">
+      <c r="R11" s="40"/>
+      <c r="S11" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="T11" s="131"/>
-      <c r="U11" s="132"/>
+      <c r="T11" s="128"/>
+      <c r="U11" s="129"/>
     </row>
     <row r="12" spans="1:21" ht="21" customHeight="1">
-      <c r="A12" s="55"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="139"/>
-      <c r="G12" s="140"/>
-      <c r="H12" s="139"/>
-      <c r="I12" s="140"/>
-      <c r="J12" s="139"/>
-      <c r="K12" s="140"/>
-      <c r="L12" s="139"/>
-      <c r="M12" s="140"/>
-      <c r="N12" s="139"/>
-      <c r="O12" s="140"/>
-      <c r="P12" s="29"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="77"/>
+      <c r="K12" s="78"/>
+      <c r="L12" s="77"/>
+      <c r="M12" s="78"/>
+      <c r="N12" s="77"/>
+      <c r="O12" s="78"/>
+      <c r="P12" s="28"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="129"/>
-      <c r="S12" s="133" t="s">
+      <c r="R12" s="70"/>
+      <c r="S12" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="T12" s="131"/>
-      <c r="U12" s="132"/>
+      <c r="T12" s="128"/>
+      <c r="U12" s="129"/>
     </row>
     <row r="13" spans="1:21" ht="21" customHeight="1">
-      <c r="A13" s="55"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="29"/>
+      <c r="A13" s="83"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="28"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="130"/>
-      <c r="S13" s="133" t="s">
+      <c r="R13" s="71"/>
+      <c r="S13" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="T13" s="131"/>
-      <c r="U13" s="132"/>
+      <c r="T13" s="128"/>
+      <c r="U13" s="129"/>
     </row>
     <row r="14" spans="1:21" ht="21" customHeight="1" thickBot="1">
-      <c r="A14" s="55"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="29"/>
+      <c r="A14" s="83"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="28"/>
       <c r="Q14" s="1"/>
-      <c r="R14" s="143"/>
-      <c r="S14" s="144" t="s">
+      <c r="R14" s="80"/>
+      <c r="S14" s="124" t="s">
         <v>25</v>
       </c>
-      <c r="T14" s="145"/>
-      <c r="U14" s="146"/>
+      <c r="T14" s="125"/>
+      <c r="U14" s="126"/>
     </row>
     <row r="15" spans="1:21" ht="21" customHeight="1">
-      <c r="A15" s="55"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="27"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="29"/>
+      <c r="A15" s="83"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="28"/>
       <c r="Q15" s="1"/>
-      <c r="R15" s="142"/>
-      <c r="S15" s="141"/>
-      <c r="T15" s="141"/>
-      <c r="U15" s="141"/>
+      <c r="R15" s="79"/>
+      <c r="S15" s="123"/>
+      <c r="T15" s="123"/>
+      <c r="U15" s="123"/>
     </row>
     <row r="16" spans="1:21" ht="21" customHeight="1">
-      <c r="A16" s="55"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="29"/>
+      <c r="A16" s="83"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="28"/>
       <c r="Q16" s="1"/>
-      <c r="R16" s="142"/>
-      <c r="S16" s="141"/>
-      <c r="T16" s="141"/>
-      <c r="U16" s="141"/>
+      <c r="R16" s="79"/>
+      <c r="S16" s="123"/>
+      <c r="T16" s="123"/>
+      <c r="U16" s="123"/>
     </row>
     <row r="17" spans="1:21" ht="21" customHeight="1">
-      <c r="A17" s="55"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="29"/>
+      <c r="A17" s="83"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="28"/>
       <c r="Q17" s="1"/>
-      <c r="R17" s="142"/>
-      <c r="S17" s="141"/>
-      <c r="T17" s="141"/>
-      <c r="U17" s="141"/>
+      <c r="R17" s="79"/>
+      <c r="S17" s="123"/>
+      <c r="T17" s="123"/>
+      <c r="U17" s="123"/>
     </row>
     <row r="18" spans="1:21" ht="21" customHeight="1">
-      <c r="A18" s="55"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="29"/>
+      <c r="A18" s="83"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="28"/>
       <c r="Q18" s="1"/>
-      <c r="R18" s="142"/>
-      <c r="S18" s="141"/>
-      <c r="T18" s="141"/>
-      <c r="U18" s="141"/>
+      <c r="R18" s="79"/>
+      <c r="S18" s="123"/>
+      <c r="T18" s="123"/>
+      <c r="U18" s="123"/>
     </row>
     <row r="19" spans="1:21" ht="21" customHeight="1">
-      <c r="A19" s="55"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="29"/>
+      <c r="A19" s="83"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="28"/>
       <c r="Q19" s="1"/>
-      <c r="R19" s="53"/>
-      <c r="S19" s="52"/>
-      <c r="T19" s="52"/>
-      <c r="U19" s="52"/>
+      <c r="R19" s="1"/>
     </row>
     <row r="20" spans="1:21" ht="21" customHeight="1">
-      <c r="A20" s="55"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="29"/>
+      <c r="A20" s="83"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="28"/>
       <c r="Q20" s="1"/>
-      <c r="R20" s="53"/>
-      <c r="S20" s="52"/>
-      <c r="T20" s="52"/>
-      <c r="U20" s="52"/>
+      <c r="R20" s="1"/>
     </row>
     <row r="21" spans="1:21" ht="21" customHeight="1">
-      <c r="A21" s="55"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="28"/>
-      <c r="P21" s="29"/>
+      <c r="A21" s="83"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="28"/>
       <c r="Q21" s="1"/>
-      <c r="R21" s="53"/>
-      <c r="S21" s="52"/>
-      <c r="T21" s="52"/>
-      <c r="U21" s="52"/>
+      <c r="R21" s="1"/>
     </row>
     <row r="22" spans="1:21" ht="21" customHeight="1">
-      <c r="A22" s="55"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="29"/>
+      <c r="A22" s="83"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="28"/>
       <c r="Q22" s="1"/>
-      <c r="R22" s="53"/>
-      <c r="S22" s="52"/>
-      <c r="T22" s="52"/>
-      <c r="U22" s="52"/>
+      <c r="R22" s="1"/>
     </row>
     <row r="23" spans="1:21" ht="21" customHeight="1">
-      <c r="A23" s="55"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="28"/>
-      <c r="P23" s="29"/>
+      <c r="A23" s="83"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="28"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
     </row>
     <row r="24" spans="1:21" ht="21" customHeight="1">
-      <c r="A24" s="55"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="28"/>
-      <c r="P24" s="29"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="28"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
     <row r="25" spans="1:21" ht="21" customHeight="1">
-      <c r="A25" s="55"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="27"/>
-      <c r="O25" s="28"/>
-      <c r="P25" s="29"/>
+      <c r="A25" s="83"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="28"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
     </row>
     <row r="26" spans="1:21" ht="21" customHeight="1">
-      <c r="A26" s="56"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="32"/>
-      <c r="P26" s="33"/>
+      <c r="A26" s="84"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="31"/>
+      <c r="P26" s="32"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
     </row>
@@ -3772,6 +3784,10 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A26"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:G3"/>
     <mergeCell ref="R8:U9"/>
     <mergeCell ref="S18:U18"/>
     <mergeCell ref="S17:U17"/>
@@ -3782,10 +3798,6 @@
     <mergeCell ref="S12:U12"/>
     <mergeCell ref="S11:U11"/>
     <mergeCell ref="S10:U10"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A26"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:G3"/>
   </mergeCells>
   <conditionalFormatting sqref="M5">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Vertex42">
@@ -3801,10 +3813,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:U28"/>
+  <dimension ref="A1:U29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -3821,28 +3833,18 @@
     <col min="13" max="14" width="5.140625" customWidth="1"/>
     <col min="15" max="15" width="5.28515625" customWidth="1"/>
     <col min="16" max="16" width="20.28515625" customWidth="1"/>
-    <col min="18" max="18" width="31.42578125" customWidth="1"/>
+    <col min="18" max="18" width="11.140625" customWidth="1"/>
+    <col min="19" max="19" width="33.85546875" customWidth="1"/>
+    <col min="20" max="21" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="50"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="34"/>
+      <c r="P1" s="35"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="3"/>
     </row>
@@ -3866,17 +3868,17 @@
       <c r="R2" s="6"/>
     </row>
     <row r="3" spans="1:21" ht="21" customHeight="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41">
+      <c r="B3" s="110"/>
+      <c r="C3" s="111"/>
+      <c r="D3" s="112">
         <v>45065</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="43"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="114"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -3961,7 +3963,7 @@
       <c r="R5" s="15"/>
     </row>
     <row r="6" spans="1:21" ht="18" customHeight="1">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="115" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="16">
@@ -4027,7 +4029,7 @@
       <c r="R6" s="19"/>
     </row>
     <row r="7" spans="1:21" ht="18" customHeight="1" thickBot="1">
-      <c r="A7" s="45"/>
+      <c r="A7" s="116"/>
       <c r="B7" s="20">
         <f t="shared" ref="B7:O7" si="1">B6</f>
         <v>45065</v>
@@ -4089,455 +4091,474 @@
       <c r="R7" s="19"/>
     </row>
     <row r="8" spans="1:21" ht="21" customHeight="1">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="26"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="73"/>
+      <c r="N8" s="74"/>
+      <c r="O8" s="153"/>
+      <c r="P8" s="25"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="S8" s="68"/>
-      <c r="T8" s="68"/>
-      <c r="U8" s="69"/>
-    </row>
-    <row r="9" spans="1:21" ht="21" customHeight="1" thickBot="1">
-      <c r="A9" s="55"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="29"/>
+      <c r="R8" s="117" t="s">
+        <v>35</v>
+      </c>
+      <c r="S8" s="118"/>
+      <c r="T8" s="118"/>
+      <c r="U8" s="119"/>
+    </row>
+    <row r="9" spans="1:21" ht="21" customHeight="1">
+      <c r="A9" s="83"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="28"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="70"/>
-      <c r="S9" s="71"/>
-      <c r="T9" s="71"/>
-      <c r="U9" s="72"/>
+      <c r="R9" s="120"/>
+      <c r="S9" s="121"/>
+      <c r="T9" s="121"/>
+      <c r="U9" s="122"/>
     </row>
     <row r="10" spans="1:21" ht="21" customHeight="1">
-      <c r="A10" s="55"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="29"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="145"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="145"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="28"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="62"/>
-      <c r="S10" s="52"/>
-      <c r="T10" s="52"/>
-      <c r="U10" s="61"/>
+      <c r="R10" s="69"/>
+      <c r="S10" s="132" t="s">
+        <v>27</v>
+      </c>
+      <c r="T10" s="132"/>
+      <c r="U10" s="135"/>
     </row>
     <row r="11" spans="1:21" ht="21" customHeight="1">
-      <c r="A11" s="55"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="29"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="77"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="77"/>
+      <c r="M11" s="78"/>
+      <c r="N11" s="77"/>
+      <c r="O11" s="152"/>
+      <c r="P11" s="28"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="62"/>
-      <c r="S11" s="52"/>
-      <c r="T11" s="52"/>
-      <c r="U11" s="61"/>
+      <c r="R11" s="146"/>
+      <c r="S11" s="133" t="s">
+        <v>34</v>
+      </c>
+      <c r="T11" s="133"/>
+      <c r="U11" s="136"/>
     </row>
     <row r="12" spans="1:21" ht="21" customHeight="1">
-      <c r="A12" s="55"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="29"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="75"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="76"/>
+      <c r="L12" s="75"/>
+      <c r="M12" s="76"/>
+      <c r="N12" s="75"/>
+      <c r="O12" s="152"/>
+      <c r="P12" s="28"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="62"/>
-      <c r="S12" s="52"/>
-      <c r="T12" s="52"/>
-      <c r="U12" s="61"/>
+      <c r="R12" s="147"/>
+      <c r="S12" s="133"/>
+      <c r="T12" s="133"/>
+      <c r="U12" s="136"/>
     </row>
     <row r="13" spans="1:21" ht="21" customHeight="1">
-      <c r="A13" s="55"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="29"/>
+      <c r="A13" s="83"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="148"/>
+      <c r="H13" s="149"/>
+      <c r="I13" s="148"/>
+      <c r="J13" s="149"/>
+      <c r="K13" s="148"/>
+      <c r="L13" s="149"/>
+      <c r="M13" s="148"/>
+      <c r="N13" s="149"/>
+      <c r="O13" s="152"/>
+      <c r="P13" s="28"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="63"/>
-      <c r="S13" s="52"/>
-      <c r="T13" s="52"/>
-      <c r="U13" s="61"/>
+      <c r="R13" s="42"/>
+      <c r="S13" s="132" t="s">
+        <v>28</v>
+      </c>
+      <c r="T13" s="132"/>
+      <c r="U13" s="135"/>
     </row>
     <row r="14" spans="1:21" ht="21" customHeight="1">
-      <c r="A14" s="55"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="29"/>
+      <c r="A14" s="83"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="150"/>
+      <c r="H14" s="151"/>
+      <c r="I14" s="150"/>
+      <c r="J14" s="151"/>
+      <c r="K14" s="150"/>
+      <c r="L14" s="151"/>
+      <c r="M14" s="150"/>
+      <c r="N14" s="151"/>
+      <c r="O14" s="152"/>
+      <c r="P14" s="28"/>
       <c r="Q14" s="1"/>
-      <c r="R14" s="63"/>
-      <c r="S14" s="52"/>
-      <c r="T14" s="52"/>
-      <c r="U14" s="61"/>
+      <c r="R14" s="71"/>
+      <c r="S14" s="134" t="s">
+        <v>29</v>
+      </c>
+      <c r="T14" s="134"/>
+      <c r="U14" s="137"/>
     </row>
     <row r="15" spans="1:21" ht="21" customHeight="1">
-      <c r="A15" s="55"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="27"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="29"/>
+      <c r="A15" s="83"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="58"/>
+      <c r="P15" s="28"/>
       <c r="Q15" s="1"/>
-      <c r="R15" s="63"/>
-      <c r="S15" s="52"/>
-      <c r="T15" s="52"/>
-      <c r="U15" s="61"/>
+      <c r="R15" s="141"/>
+      <c r="S15" s="134" t="s">
+        <v>30</v>
+      </c>
+      <c r="T15" s="134"/>
+      <c r="U15" s="137"/>
     </row>
     <row r="16" spans="1:21" ht="21" customHeight="1">
-      <c r="A16" s="55"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="29"/>
+      <c r="A16" s="83"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="28"/>
       <c r="Q16" s="1"/>
-      <c r="R16" s="63"/>
-      <c r="S16" s="52"/>
-      <c r="T16" s="52"/>
-      <c r="U16" s="61"/>
+      <c r="R16" s="142"/>
+      <c r="S16" s="134" t="s">
+        <v>31</v>
+      </c>
+      <c r="T16" s="134"/>
+      <c r="U16" s="137"/>
     </row>
     <row r="17" spans="1:21" ht="21" customHeight="1">
-      <c r="A17" s="55"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="29"/>
+      <c r="A17" s="83"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="28"/>
       <c r="Q17" s="1"/>
-      <c r="R17" s="63"/>
-      <c r="S17" s="52"/>
-      <c r="T17" s="52"/>
-      <c r="U17" s="61"/>
-    </row>
-    <row r="18" spans="1:21" ht="21" customHeight="1">
-      <c r="A18" s="55"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="29"/>
+      <c r="R17" s="143"/>
+      <c r="S17" s="134" t="s">
+        <v>32</v>
+      </c>
+      <c r="T17" s="134"/>
+      <c r="U17" s="137"/>
+    </row>
+    <row r="18" spans="1:21" ht="21" customHeight="1" thickBot="1">
+      <c r="A18" s="83"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="28"/>
       <c r="Q18" s="1"/>
-      <c r="R18" s="63"/>
-      <c r="S18" s="52"/>
-      <c r="T18" s="52"/>
-      <c r="U18" s="61"/>
+      <c r="R18" s="144"/>
+      <c r="S18" s="138" t="s">
+        <v>33</v>
+      </c>
+      <c r="T18" s="139"/>
+      <c r="U18" s="140"/>
     </row>
     <row r="19" spans="1:21" ht="21" customHeight="1">
-      <c r="A19" s="55"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="29"/>
+      <c r="A19" s="83"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="28"/>
       <c r="Q19" s="1"/>
-      <c r="R19" s="63"/>
-      <c r="S19" s="52"/>
-      <c r="T19" s="52"/>
-      <c r="U19" s="61"/>
+      <c r="R19" s="131"/>
+      <c r="S19" s="130"/>
+      <c r="T19" s="130"/>
+      <c r="U19" s="130"/>
     </row>
     <row r="20" spans="1:21" ht="21" customHeight="1">
-      <c r="A20" s="55"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="29"/>
+      <c r="A20" s="83"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="28"/>
       <c r="Q20" s="1"/>
-      <c r="R20" s="63"/>
-      <c r="S20" s="52"/>
-      <c r="T20" s="52"/>
-      <c r="U20" s="61"/>
+      <c r="R20" s="131"/>
+      <c r="S20" s="130"/>
+      <c r="T20" s="130"/>
+      <c r="U20" s="130"/>
     </row>
     <row r="21" spans="1:21" ht="21" customHeight="1">
-      <c r="A21" s="55"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="28"/>
-      <c r="P21" s="29"/>
+      <c r="A21" s="83"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="28"/>
       <c r="Q21" s="1"/>
-      <c r="R21" s="63"/>
-      <c r="S21" s="52"/>
-      <c r="T21" s="52"/>
-      <c r="U21" s="61"/>
-    </row>
-    <row r="22" spans="1:21" ht="21" customHeight="1" thickBot="1">
-      <c r="A22" s="55"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="29"/>
+      <c r="R21" s="131"/>
+      <c r="S21" s="130"/>
+      <c r="T21" s="130"/>
+      <c r="U21" s="130"/>
+    </row>
+    <row r="22" spans="1:21" ht="21" customHeight="1">
+      <c r="A22" s="83"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="28"/>
       <c r="Q22" s="1"/>
-      <c r="R22" s="64"/>
-      <c r="S22" s="65"/>
-      <c r="T22" s="65"/>
-      <c r="U22" s="66"/>
+      <c r="R22" s="131"/>
+      <c r="S22" s="130"/>
+      <c r="T22" s="130"/>
+      <c r="U22" s="130"/>
     </row>
     <row r="23" spans="1:21" ht="21" customHeight="1">
-      <c r="A23" s="55"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="28"/>
-      <c r="P23" s="29"/>
+      <c r="A23" s="83"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="28"/>
       <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
+      <c r="R23" s="131"/>
+      <c r="S23" s="130"/>
+      <c r="T23" s="130"/>
+      <c r="U23" s="130"/>
     </row>
     <row r="24" spans="1:21" ht="21" customHeight="1">
-      <c r="A24" s="55"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="28"/>
-      <c r="P24" s="29"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="28"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
     <row r="25" spans="1:21" ht="21" customHeight="1">
-      <c r="A25" s="55"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="27"/>
-      <c r="O25" s="28"/>
-      <c r="P25" s="29"/>
+      <c r="A25" s="83"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="28"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
     </row>
     <row r="26" spans="1:21" ht="21" customHeight="1">
-      <c r="A26" s="56"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="32"/>
-      <c r="P26" s="33"/>
+      <c r="A26" s="83"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="28"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
     </row>
     <row r="27" spans="1:21" ht="21" customHeight="1">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
+      <c r="A27" s="84"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="31"/>
+      <c r="P27" s="32"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="1:21" ht="21" hidden="1" customHeight="1">
+    <row r="28" spans="1:21" ht="21" customHeight="1">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -4553,16 +4574,45 @@
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
     </row>
+    <row r="29" spans="1:21" ht="21" hidden="1" customHeight="1">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A8:A26"/>
+  <mergeCells count="14">
+    <mergeCell ref="A8:A27"/>
     <mergeCell ref="R8:U9"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D3:G3"/>
     <mergeCell ref="A6:A7"/>
+    <mergeCell ref="S17:U17"/>
+    <mergeCell ref="S16:U16"/>
+    <mergeCell ref="S15:U15"/>
+    <mergeCell ref="S14:U14"/>
+    <mergeCell ref="S13:U13"/>
+    <mergeCell ref="S10:U10"/>
+    <mergeCell ref="S11:U12"/>
+    <mergeCell ref="S18:U18"/>
+    <mergeCell ref="R11:R12"/>
   </mergeCells>
   <conditionalFormatting sqref="M5">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Vertex42">

</xml_diff>